<commit_message>
Update Zeiterfassung KW 13
</commit_message>
<xml_diff>
--- a/Privat/Arbeit/Zeiterfassung_2024.xlsx
+++ b/Privat/Arbeit/Zeiterfassung_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npawelka\Desktop\repo\Home\Privat\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17B13C3-2DD5-4552-B525-50521A9FA01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54445178-7DA4-468F-B08E-48C74DF63866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="48">
   <si>
     <t>Datum</t>
   </si>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="C14" s="17">
         <f>März!L3</f>
-        <v>0.45833333333333304</v>
+        <v>0.54999999999999971</v>
       </c>
       <c r="D14" s="1">
         <f>März!L7</f>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C25" s="18">
         <f>SUM(C12:C23)+C4</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="D25" s="13">
         <f>SUM(D12:D23)</f>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -2484,7 +2484,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -3419,7 +3419,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -4330,7 +4330,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="20" t="s">
         <v>45</v>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -6235,7 +6235,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -12623,7 +12623,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12730,7 +12730,7 @@
       </c>
       <c r="L3" s="17">
         <f>I34</f>
-        <v>0.45833333333333304</v>
+        <v>0.54999999999999971</v>
       </c>
       <c r="O3" s="23" t="s">
         <v>43</v>
@@ -12797,7 +12797,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -13390,16 +13390,22 @@
         <f t="shared" si="3"/>
         <v>Arbeit</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="E26" s="16">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F26" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G26" s="16">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H26" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="I26" s="17">
+        <f t="shared" si="1"/>
+        <v>0.19166666666666662</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -13410,20 +13416,23 @@
         <f t="shared" si="2"/>
         <v>Dienstag</v>
       </c>
-      <c r="D27" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>Arbeit</v>
-      </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="D27" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0</v>
+      </c>
+      <c r="F27" s="16">
+        <v>0</v>
+      </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="I27" s="17">
+        <f t="shared" si="1"/>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -13482,9 +13491,8 @@
         <f t="shared" si="2"/>
         <v>Freitag</v>
       </c>
-      <c r="D30" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>Arbeit</v>
+      <c r="D30" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -13555,15 +13563,15 @@
       <c r="F34" s="26"/>
       <c r="G34" s="29">
         <f>SUM(G2:G32)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.10416666666666666</v>
       </c>
       <c r="H34" s="29">
         <f>SUM(H2:H32)</f>
-        <v>1.958333333333333</v>
+        <v>2.2499999999999996</v>
       </c>
       <c r="I34" s="28">
         <f>SUM(I2:I32)</f>
-        <v>0.45833333333333304</v>
+        <v>0.54999999999999971</v>
       </c>
     </row>
   </sheetData>
@@ -13790,7 +13798,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -14701,7 +14709,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -15637,7 +15645,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -16548,7 +16556,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>
@@ -17483,7 +17491,7 @@
       </c>
       <c r="L5" s="17">
         <f>Übersicht!C25</f>
-        <v>0.51041666666666641</v>
+        <v>0.60208333333333308</v>
       </c>
       <c r="O5" s="23" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Zeiterfassung KW 20 Teil 1
</commit_message>
<xml_diff>
--- a/Privat/Arbeit/Zeiterfassung_2024.xlsx
+++ b/Privat/Arbeit/Zeiterfassung_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npawelka\Desktop\repo\Home\Privat\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5430A344-4F5A-40BE-9261-D660E267A008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187CEF82-1382-41F6-9035-E0810780F6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rbo4xuPTTOkY/xEJa0tiapcXR+ldBHWm5hXsVmeGY9Jj5YL0tEljowGf7bSUcDVujfPfBnB1zbs5S4t6qCpzrA==" workbookSaltValue="OrWd5cud9Ev5I/HlVYVjUg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E11)-SUM(Gesamt!J2:J11)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E12)-SUM(Gesamt!J2:J12)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E13)-SUM(Gesamt!J2:J13)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -6932,7 +6932,7 @@
       </c>
       <c r="E6" s="7">
         <f ca="1">Mai!M5</f>
-        <v>0.50000000000000178</v>
+        <v>0.50000000000000089</v>
       </c>
       <c r="F6" s="8">
         <f>Mai!M9</f>
@@ -6944,7 +6944,7 @@
       </c>
       <c r="H6" s="7">
         <f>Mai!M17</f>
-        <v>8.5000000000000018</v>
+        <v>20.5</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7">
@@ -7172,7 +7172,7 @@
       </c>
       <c r="E15" s="7">
         <f ca="1">SUM(E2:E13)</f>
-        <v>17.000000000000007</v>
+        <v>17.000000000000004</v>
       </c>
       <c r="F15" s="8">
         <f>SUM(F2:F13)</f>
@@ -7184,7 +7184,7 @@
       </c>
       <c r="H15" s="7">
         <f>SUM(H2:H13)</f>
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
@@ -7214,7 +7214,7 @@
       </c>
       <c r="E17" s="7">
         <f ca="1">SUM(E2:E13)+B9-J15</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -10691,7 +10691,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10861,7 +10861,7 @@
       </c>
       <c r="M5" s="27">
         <f ca="1">SUM(I2:I32)</f>
-        <v>0.50000000000000178</v>
+        <v>0.50000000000000089</v>
       </c>
       <c r="N5" s="36"/>
       <c r="P5" s="7"/>
@@ -10926,7 +10926,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E6)-SUM(Gesamt!J2:J6)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -10964,17 +10964,23 @@
         <f t="shared" si="0"/>
         <v>Mi</v>
       </c>
+      <c r="D9" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="G9" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.9999999999999991</v>
       </c>
       <c r="H9" s="27">
         <f ca="1">IF(P9&lt;&gt;"",P9,IF(OR(C9="Feiertag",A9&lt;Gesamt!$B$11,A9&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A9,2)+19)))</f>
         <v>4</v>
       </c>
       <c r="I9" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-8.8817841970012523E-16</v>
       </c>
       <c r="J9" s="7"/>
       <c r="L9" s="1" t="s">
@@ -11107,16 +11113,25 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="D14" s="24">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F14" s="24">
+        <v>3.125E-2</v>
+      </c>
       <c r="G14" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H14" s="27">
         <f ca="1">IF(P14&lt;&gt;"",P14,IF(OR(C14="Feiertag",A14&lt;Gesamt!$B$11,A14&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A14,2)+19)))</f>
         <v>8</v>
       </c>
       <c r="I14" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="J14" s="7"/>
@@ -11205,7 +11220,7 @@
       </c>
       <c r="M17" s="27">
         <f>SUM(G2:G32)</f>
-        <v>8.5000000000000018</v>
+        <v>20.5</v>
       </c>
       <c r="N17" s="36"/>
       <c r="P17" s="7"/>
@@ -11895,7 +11910,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E7)-SUM(Gesamt!J2:J7)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -12847,7 +12862,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E8)-SUM(Gesamt!J2:J8)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -13816,7 +13831,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E9)-SUM(Gesamt!J2:J9)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -14785,7 +14800,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E10)-SUM(Gesamt!J2:J10)</f>
-        <v>18.250000000000007</v>
+        <v>18.250000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>

</xml_diff>

<commit_message>
Update Zeiterfassung KW 26
</commit_message>
<xml_diff>
--- a/Privat/Arbeit/Zeiterfassung_2024.xlsx
+++ b/Privat/Arbeit/Zeiterfassung_2024.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npawelka\Desktop\repo\Home\Privat\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142D7FF3-3F90-4776-B915-FAC982A754A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1FFD96-D3D9-44AF-85C8-B362F72F5D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rbo4xuPTTOkY/xEJa0tiapcXR+ldBHWm5hXsVmeGY9Jj5YL0tEljowGf7bSUcDVujfPfBnB1zbs5S4t6qCpzrA==" workbookSaltValue="OrWd5cud9Ev5I/HlVYVjUg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Januar" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="69">
   <si>
     <t>Datum</t>
   </si>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E11)-SUM(Gesamt!J2:J11)</f>
-        <v>10.750000000000004</v>
+        <v>-5.9999999999999964</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -4318,7 +4318,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G11)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -5063,7 +5063,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E12)-SUM(Gesamt!J2:J12)</f>
-        <v>10.750000000000004</v>
+        <v>-5.9999999999999964</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G12)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E13)-SUM(Gesamt!J2:J13)</f>
-        <v>10.750000000000004</v>
+        <v>-5.9999999999999964</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -6238,7 +6238,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G13)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="E7" s="7">
         <f ca="1">Juni!M5</f>
-        <v>-15.75</v>
+        <v>-16.5</v>
       </c>
       <c r="F7" s="8">
         <f>Juni!M9</f>
@@ -6978,7 +6978,7 @@
       </c>
       <c r="H7" s="7">
         <f>Juni!M17</f>
-        <v>24.25</v>
+        <v>31.5</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7">
@@ -6993,8 +6993,8 @@
         <v>15</v>
       </c>
       <c r="E8" s="7">
-        <f>Juli!M5</f>
-        <v>0</v>
+        <f ca="1">Juli!M5</f>
+        <v>-16</v>
       </c>
       <c r="F8" s="8">
         <f>Juli!M9</f>
@@ -7002,11 +7002,11 @@
       </c>
       <c r="G8" s="2">
         <f>Juli!M13</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H8" s="7">
-        <f>Juli!M17</f>
-        <v>0</v>
+        <f ca="1">Juli!M17</f>
+        <v>28</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7">
@@ -7033,11 +7033,11 @@
       </c>
       <c r="G9" s="2">
         <f>August!M13</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="7">
-        <f>August!M17</f>
-        <v>0</v>
+        <f ca="1">August!M17</f>
+        <v>12</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7">
@@ -7172,7 +7172,7 @@
       </c>
       <c r="E15" s="7">
         <f ca="1">SUM(E2:E13)</f>
-        <v>9.5000000000000036</v>
+        <v>-7.2499999999999964</v>
       </c>
       <c r="F15" s="8">
         <f>SUM(F2:F13)</f>
@@ -7180,11 +7180,11 @@
       </c>
       <c r="G15" s="2">
         <f>SUM(G2:G13)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H15" s="7">
-        <f>SUM(H2:H13)</f>
-        <v>185.5</v>
+        <f ca="1">SUM(H2:H13)</f>
+        <v>232.75</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
@@ -7214,7 +7214,7 @@
       </c>
       <c r="E17" s="7">
         <f ca="1">SUM(E2:E13)+B9-J15</f>
-        <v>10.750000000000004</v>
+        <v>-5.9999999999999964</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -7230,7 +7230,7 @@
       </c>
       <c r="G18" s="2">
         <f>B5+B7-G15</f>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -11728,8 +11728,8 @@
   </sheetPr>
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11905,7 +11905,7 @@
       </c>
       <c r="M5" s="27">
         <f ca="1">SUM(I2:I32)</f>
-        <v>-15.75</v>
+        <v>-16.5</v>
       </c>
       <c r="N5" s="36"/>
       <c r="P5" s="7"/>
@@ -11964,7 +11964,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E7)-SUM(Gesamt!J2:J7)</f>
-        <v>10.750000000000004</v>
+        <v>10.000000000000004</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -12255,7 +12255,7 @@
       </c>
       <c r="M17" s="27">
         <f>SUM(G2:G32)</f>
-        <v>24.25</v>
+        <v>31.5</v>
       </c>
       <c r="N17" s="36"/>
       <c r="P17" s="7"/>
@@ -12486,17 +12486,26 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="D25" s="24">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="E25" s="24">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F25" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G25" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.2500000000000009</v>
       </c>
       <c r="H25" s="27">
         <f ca="1">IF(P25&lt;&gt;"",P25,IF(OR(C25="Feiertag",A25&lt;Gesamt!$B$11,A25&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A25,2)+19)))</f>
         <v>8</v>
       </c>
       <c r="I25" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.74999999999999911</v>
       </c>
       <c r="J25" s="7"/>
       <c r="L25" s="6" t="s">
@@ -12719,8 +12728,8 @@
   </sheetPr>
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12844,6 +12853,9 @@
         <f t="shared" si="0"/>
         <v>Mi</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="G4" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -12853,8 +12865,8 @@
         <v>4</v>
       </c>
       <c r="I4" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-4</v>
       </c>
       <c r="J4" s="7"/>
       <c r="N4" s="36"/>
@@ -12886,8 +12898,8 @@
         <v>8</v>
       </c>
       <c r="M5" s="27">
-        <f>SUM(I2:I32)</f>
-        <v>0</v>
+        <f ca="1">SUM(I2:I32)</f>
+        <v>-16</v>
       </c>
       <c r="N5" s="36"/>
       <c r="P5" s="7"/>
@@ -12943,7 +12955,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E8)-SUM(Gesamt!J2:J8)</f>
-        <v>10.750000000000004</v>
+        <v>-5.9999999999999964</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -12981,9 +12993,12 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
       </c>
       <c r="H9" s="27">
         <f ca="1">IF(P9&lt;&gt;"",P9,IF(OR(C9="Feiertag",A9&lt;Gesamt!$B$11,A9&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A9,2)+19)))</f>
@@ -13037,6 +13052,9 @@
         <f t="shared" si="0"/>
         <v>Mi</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="G11" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -13046,8 +13064,8 @@
         <v>4</v>
       </c>
       <c r="I11" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-4</v>
       </c>
       <c r="J11" s="7"/>
       <c r="L11" s="1" t="s">
@@ -13111,7 +13129,7 @@
       </c>
       <c r="M13">
         <f>COUNTIF(C2:C32, "Urlaub")+COUNTIF(C2:C32,"Urlaub halber Tag")/2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N13" s="36"/>
       <c r="P13" s="7"/>
@@ -13167,7 +13185,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G8)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -13180,9 +13198,12 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G16" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
       </c>
       <c r="H16" s="27">
         <f ca="1">IF(P16&lt;&gt;"",P16,IF(OR(C16="Feiertag",A16&lt;Gesamt!$B$11,A16&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A16,2)+19)))</f>
@@ -13221,8 +13242,8 @@
         <v>50</v>
       </c>
       <c r="M17" s="27">
-        <f>SUM(G2:G32)</f>
-        <v>0</v>
+        <f ca="1">SUM(G2:G32)</f>
+        <v>28</v>
       </c>
       <c r="N17" s="36"/>
       <c r="P17" s="7"/>
@@ -13235,6 +13256,9 @@
         <f t="shared" si="0"/>
         <v>Mi</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="G18" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -13244,8 +13268,8 @@
         <v>4</v>
       </c>
       <c r="I18" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-4</v>
       </c>
       <c r="J18" s="7"/>
       <c r="N18" s="36"/>
@@ -13441,6 +13465,9 @@
         <f t="shared" si="0"/>
         <v>Mi</v>
       </c>
+      <c r="C25" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="G25" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -13450,8 +13477,8 @@
         <v>4</v>
       </c>
       <c r="I25" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-4</v>
       </c>
       <c r="J25" s="7"/>
       <c r="L25" s="6" t="s">
@@ -13582,9 +13609,12 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="C30" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G30" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
       </c>
       <c r="H30" s="27">
         <f ca="1">IF(P30&lt;&gt;"",P30,IF(OR(C30="Feiertag",A30&lt;Gesamt!$B$11,A30&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A30,2)+19)))</f>
@@ -13630,9 +13660,12 @@
         <f t="shared" si="0"/>
         <v>Mi</v>
       </c>
+      <c r="C32" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G32" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="H32" s="27">
         <f ca="1">IF(P32&lt;&gt;"",P32,IF(OR(C32="Feiertag",A32&lt;Gesamt!$B$11,A32&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A32,2)+19)))</f>
@@ -13689,7 +13722,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13869,9 +13902,12 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
       </c>
       <c r="H6" s="27">
         <f ca="1">IF(P6&lt;&gt;"",P6,IF(OR(C6="Feiertag",A6&lt;Gesamt!$B$11,A6&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A6,2)+19)))</f>
@@ -13912,7 +13948,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E9)-SUM(Gesamt!J2:J9)</f>
-        <v>10.750000000000004</v>
+        <v>-5.9999999999999964</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -13925,9 +13961,12 @@
         <f t="shared" si="0"/>
         <v>Mi</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G8" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="H8" s="27">
         <f ca="1">IF(P8&lt;&gt;"",P8,IF(OR(C8="Feiertag",A8&lt;Gesamt!$B$11,A8&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A8,2)+19)))</f>
@@ -14080,7 +14119,7 @@
       </c>
       <c r="M13">
         <f>COUNTIF(C2:C32, "Urlaub")+COUNTIF(C2:C32,"Urlaub halber Tag")/2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="36"/>
       <c r="P13" s="7"/>
@@ -14136,7 +14175,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G9)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -14190,8 +14229,8 @@
         <v>50</v>
       </c>
       <c r="M17" s="27">
-        <f>SUM(G2:G32)</f>
-        <v>0</v>
+        <f ca="1">SUM(G2:G32)</f>
+        <v>12</v>
       </c>
       <c r="N17" s="36"/>
       <c r="P17" s="7"/>
@@ -14881,7 +14920,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E10)-SUM(Gesamt!J2:J10)</f>
-        <v>10.750000000000004</v>
+        <v>-5.9999999999999964</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -15106,7 +15145,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G10)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>

</xml_diff>

<commit_message>
Update Arbeitszeit KW 33
</commit_message>
<xml_diff>
--- a/Privat/Arbeit/Zeiterfassung_2024.xlsx
+++ b/Privat/Arbeit/Zeiterfassung_2024.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npawelka\Desktop\repo\Home\Privat\Arbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59F4246-4AB5-4268-9A23-147524B75353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFE5699-6532-404F-A068-58E6D0E579E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Rbo4xuPTTOkY/xEJa0tiapcXR+ldBHWm5hXsVmeGY9Jj5YL0tEljowGf7bSUcDVujfPfBnB1zbs5S4t6qCpzrA==" workbookSaltValue="OrWd5cud9Ev5I/HlVYVjUg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Januar" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="71">
   <si>
     <t>Datum</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>Nicolas Pawelka</t>
+  </si>
+  <si>
+    <t>Vorlesungsstart</t>
+  </si>
+  <si>
+    <t>Lissabon</t>
   </si>
 </sst>
 </file>
@@ -3351,7 +3357,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-Gesamt!G2</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -4094,7 +4100,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E11)-SUM(Gesamt!J2:J11)</f>
-        <v>-5.9999999999999964</v>
+        <v>-13.999999999999996</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -4318,7 +4324,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G11)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -5063,7 +5069,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E12)-SUM(Gesamt!J2:J12)</f>
-        <v>-5.9999999999999964</v>
+        <v>-13.999999999999996</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -5287,7 +5293,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G12)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -6014,7 +6020,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E13)-SUM(Gesamt!J2:J13)</f>
-        <v>-5.9999999999999964</v>
+        <v>-13.999999999999996</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -6238,7 +6244,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G13)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -6760,7 +6766,7 @@
   <dimension ref="A1:Z44"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6897,7 +6903,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>12</v>
@@ -6994,7 +7000,7 @@
       </c>
       <c r="E8" s="7">
         <f ca="1">Juli!M5</f>
-        <v>-16</v>
+        <v>-24</v>
       </c>
       <c r="F8" s="8">
         <f>Juli!M9</f>
@@ -7024,7 +7030,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="7">
-        <f>August!M5</f>
+        <f ca="1">August!M5</f>
         <v>0</v>
       </c>
       <c r="F9" s="8">
@@ -7037,7 +7043,7 @@
       </c>
       <c r="H9" s="7">
         <f ca="1">August!M17</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7">
@@ -7172,7 +7178,7 @@
       </c>
       <c r="E15" s="7">
         <f ca="1">SUM(E2:E13)</f>
-        <v>-7.2499999999999964</v>
+        <v>-15.249999999999996</v>
       </c>
       <c r="F15" s="8">
         <f>SUM(F2:F13)</f>
@@ -7184,7 +7190,7 @@
       </c>
       <c r="H15" s="7">
         <f ca="1">SUM(H2:H13)</f>
-        <v>240.75</v>
+        <v>248.75</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
@@ -7214,7 +7220,7 @@
       </c>
       <c r="E17" s="7">
         <f ca="1">SUM(E2:E13)+B9-J15</f>
-        <v>-5.9999999999999964</v>
+        <v>-13.999999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -7230,7 +7236,7 @@
       </c>
       <c r="G18" s="2">
         <f>B5+B7-G15</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -8141,7 +8147,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G3)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -9113,7 +9119,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G4)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -10145,7 +10151,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G5)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -11165,7 +11171,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G6)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -12200,7 +12206,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G7)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -12728,8 +12734,8 @@
   </sheetPr>
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12908,7 +12914,7 @@
       </c>
       <c r="M5" s="27">
         <f ca="1">SUM(I2:I32)</f>
-        <v>-16</v>
+        <v>-24</v>
       </c>
       <c r="N5" s="36"/>
       <c r="P5" s="7"/>
@@ -12964,7 +12970,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E8)-SUM(Gesamt!J2:J8)</f>
-        <v>-5.9999999999999964</v>
+        <v>-13.999999999999996</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -13194,7 +13200,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G8)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -13412,6 +13418,9 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="G23" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -13421,8 +13430,8 @@
         <v>8</v>
       </c>
       <c r="I23" s="27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-8</v>
       </c>
       <c r="J23" s="7"/>
       <c r="L23" s="6" t="s">
@@ -13730,8 +13739,8 @@
   </sheetPr>
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13897,7 +13906,7 @@
         <v>8</v>
       </c>
       <c r="M5" s="27">
-        <f>SUM(I2:I32)</f>
+        <f ca="1">SUM(I2:I32)</f>
         <v>0</v>
       </c>
       <c r="N5" s="36"/>
@@ -13957,7 +13966,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E9)-SUM(Gesamt!J2:J9)</f>
-        <v>-5.9999999999999964</v>
+        <v>-13.999999999999996</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -14110,16 +14119,25 @@
         <f t="shared" si="0"/>
         <v>Mo</v>
       </c>
+      <c r="D13" s="24">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F13" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G13" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H13" s="27">
         <f ca="1">IF(P13&lt;&gt;"",P13,IF(OR(C13="Feiertag",A13&lt;Gesamt!$B$11,A13&gt;Gesamt!$B$13,),0,INDIRECT("M"&amp;WEEKDAY(A13,2)+19)))</f>
         <v>8</v>
       </c>
       <c r="I13" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="J13" s="7"/>
@@ -14184,7 +14202,7 @@
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G9)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -14239,7 +14257,7 @@
       </c>
       <c r="M17" s="27">
         <f ca="1">SUM(G2:G32)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="N17" s="36"/>
       <c r="P17" s="7"/>
@@ -14706,7 +14724,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="P2" sqref="P2:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14929,7 +14947,7 @@
       </c>
       <c r="M7" s="27">
         <f ca="1">Gesamt!B9+SUM(Gesamt!E2:E10)-SUM(Gesamt!J2:J10)</f>
-        <v>-5.9999999999999964</v>
+        <v>-13.999999999999996</v>
       </c>
       <c r="N7" s="36"/>
       <c r="P7" s="7"/>
@@ -15036,7 +15054,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="L11" s="1" t="s">
         <v>57</v>
       </c>
@@ -15067,7 +15087,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="7"/>
+      <c r="J12" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="L12" s="25"/>
       <c r="N12" s="36"/>
       <c r="P12" s="7"/>
@@ -15092,7 +15114,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="L13" s="1" t="s">
         <v>26</v>
       </c>
@@ -15123,7 +15147,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="7"/>
+      <c r="J14" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="L14" s="25"/>
       <c r="N14" s="36"/>
       <c r="P14" s="7"/>
@@ -15148,13 +15174,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J15" s="7"/>
+      <c r="J15" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="L15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="M15">
         <f>Gesamt!B5+Gesamt!B7-SUM(Gesamt!G2:G10)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N15" s="36"/>
       <c r="P15" s="7"/>
@@ -15179,7 +15207,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="7"/>
+      <c r="J16" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="N16" s="36"/>
       <c r="P16" s="7"/>
     </row>
@@ -15203,7 +15233,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="7"/>
+      <c r="J17" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="L17" s="1" t="s">
         <v>50</v>
       </c>
@@ -15234,7 +15266,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J18" s="7"/>
+      <c r="J18" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="N18" s="36"/>
       <c r="P18" s="7"/>
     </row>
@@ -15258,7 +15292,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J19" s="7"/>
+      <c r="J19" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="L19" s="13" t="s">
         <v>6</v>
       </c>
@@ -15352,7 +15388,6 @@
         <v>45</v>
       </c>
       <c r="M22" s="7">
-        <f>Gesamt!C32</f>
         <v>4</v>
       </c>
       <c r="N22" s="36"/>
@@ -15440,7 +15475,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="7"/>
+      <c r="J25" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="L25" s="6" t="s">
         <v>48</v>
       </c>

</xml_diff>